<commit_message>
Added plot functions, fixed wrong value in thruster positions, added gifs to temp, modified commandToForce for tunability
</commit_message>
<xml_diff>
--- a/src/inits/mission file archive/missionfile_FF_v1.xlsx
+++ b/src/inits/mission file archive/missionfile_FF_v1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Cyclone Robosub\SimulinkPlant\src\inits\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Cyclone Robosub\SimulinkPlant\src\inits\mission file archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD95915-18A9-46FA-886A-6F65975227C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9FE3BB-0187-410D-9F02-03410D066483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -366,7 +366,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,7 +397,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>1</v>

</xml_diff>